<commit_message>
fix scale and colors
</commit_message>
<xml_diff>
--- a/20240411circuiti3/circuiti3.xlsx
+++ b/20240411circuiti3/circuiti3.xlsx
@@ -3,19 +3,20 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="RC" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="RL" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="R_RLC" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="L_RLC" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t xml:space="preserve">R (kohm)</t>
   </si>
@@ -91,6 +92,27 @@
   <si>
     <t>sigmaF_LC</t>
   </si>
+  <si>
+    <t>RL</t>
+  </si>
+  <si>
+    <t>Vinpp</t>
+  </si>
+  <si>
+    <t>VLpp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">faseL  (deg)</t>
+  </si>
+  <si>
+    <t>sigmaV_inpp</t>
+  </si>
+  <si>
+    <t>sigmaV_Lpp</t>
+  </si>
+  <si>
+    <t>sigmaVL</t>
+  </si>
 </sst>
 </file>
 
@@ -99,7 +121,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11.000000"/>
       <color theme="1"/>
@@ -112,8 +134,14 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11.000000"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -124,6 +152,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
     <fill>
@@ -154,15 +188,16 @@
       <diagonal style="none"/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf fontId="1" fillId="2" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
+    <xf fontId="2" fillId="3" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="0" fillId="3" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
     <xf fontId="0" fillId="4" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
     <xf fontId="0" fillId="5" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf fontId="0" fillId="6" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="2" xfId="0" applyNumberFormat="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="164" xfId="0" applyNumberFormat="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="2" xfId="0" applyNumberFormat="1">
@@ -174,10 +209,16 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="164" xfId="0" applyNumberFormat="1">
       <protection hidden="0" locked="1"/>
     </xf>
+    <xf fontId="0" fillId="5" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf fontId="2" fillId="3" borderId="0" numFmtId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf fontId="2" fillId="3" borderId="0" numFmtId="0" xfId="2" applyFont="1" applyFill="1">
+      <protection hidden="0" locked="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -4328,4 +4369,728 @@
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+  <sheetViews>
+    <sheetView zoomScale="100" workbookViewId="0">
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col customWidth="1" min="6" max="6" width="15.28125"/>
+    <col customWidth="1" min="9" max="9" width="13.00390625"/>
+    <col customWidth="1" min="10" max="10" width="13.7109375"/>
+    <col customWidth="1" min="11" max="11" width="12.57421875"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L1" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="7">
+        <v>9.9499999999999993</v>
+      </c>
+      <c r="B2" s="7">
+        <v>40</v>
+      </c>
+      <c r="C2" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="D2" s="6">
+        <v>5.0800000000000001</v>
+      </c>
+      <c r="E2" s="6">
+        <v>0.024</v>
+      </c>
+      <c r="F2" s="8">
+        <v>148</v>
+      </c>
+      <c r="G2" s="6">
+        <f t="shared" ref="G2:G9" si="0">D2/2</f>
+        <v>2.54</v>
+      </c>
+      <c r="H2" s="6">
+        <f t="shared" ref="H2:H9" si="1">D2/2</f>
+        <v>2.54</v>
+      </c>
+      <c r="I2" s="8">
+        <v>0.80000000000000004</v>
+      </c>
+      <c r="J2" s="8">
+        <v>0.80000000000000004</v>
+      </c>
+      <c r="K2" s="8">
+        <v>3</v>
+      </c>
+      <c r="L2">
+        <f t="shared" ref="L2:L9" si="2">I2/2</f>
+        <v>0.40000000000000002</v>
+      </c>
+      <c r="M2">
+        <f t="shared" ref="M2:M9" si="3">J2/2</f>
+        <v>0.40000000000000002</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="8">
+        <v>1</v>
+      </c>
+      <c r="D3" s="6">
+        <v>5.0800000000000001</v>
+      </c>
+      <c r="E3" s="6">
+        <v>0.080000000000000002</v>
+      </c>
+      <c r="F3" s="8">
+        <v>141</v>
+      </c>
+      <c r="G3" s="6">
+        <f t="shared" si="0"/>
+        <v>2.54</v>
+      </c>
+      <c r="H3" s="6">
+        <f t="shared" si="1"/>
+        <v>2.54</v>
+      </c>
+      <c r="I3" s="8">
+        <v>0.80000000000000004</v>
+      </c>
+      <c r="J3" s="8">
+        <v>0.80000000000000004</v>
+      </c>
+      <c r="K3" s="8">
+        <v>3</v>
+      </c>
+      <c r="L3">
+        <f t="shared" si="2"/>
+        <v>0.40000000000000002</v>
+      </c>
+      <c r="M3">
+        <f t="shared" si="3"/>
+        <v>0.40000000000000002</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="8">
+        <v>2</v>
+      </c>
+      <c r="D4" s="6">
+        <v>5.0800000000000001</v>
+      </c>
+      <c r="E4" s="6">
+        <v>0.23999999999999999</v>
+      </c>
+      <c r="F4" s="8">
+        <v>124.5</v>
+      </c>
+      <c r="G4" s="6">
+        <f t="shared" si="0"/>
+        <v>2.54</v>
+      </c>
+      <c r="H4" s="6">
+        <f t="shared" si="1"/>
+        <v>2.54</v>
+      </c>
+      <c r="I4" s="8">
+        <v>0.80000000000000004</v>
+      </c>
+      <c r="J4" s="8">
+        <v>0.80000000000000004</v>
+      </c>
+      <c r="K4" s="8">
+        <v>3</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="2"/>
+        <v>0.40000000000000002</v>
+      </c>
+      <c r="M4">
+        <f t="shared" si="3"/>
+        <v>0.40000000000000002</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="8">
+        <v>4</v>
+      </c>
+      <c r="D5" s="6">
+        <v>5.0800000000000001</v>
+      </c>
+      <c r="E5" s="6">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="F5" s="8">
+        <v>105.5</v>
+      </c>
+      <c r="G5" s="6">
+        <f t="shared" si="0"/>
+        <v>2.54</v>
+      </c>
+      <c r="H5" s="6">
+        <f t="shared" si="1"/>
+        <v>2.54</v>
+      </c>
+      <c r="I5" s="8">
+        <v>0.80000000000000004</v>
+      </c>
+      <c r="J5" s="8">
+        <v>0.80000000000000004</v>
+      </c>
+      <c r="K5" s="8">
+        <v>2</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="2"/>
+        <v>0.40000000000000002</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="3"/>
+        <v>0.40000000000000002</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="8">
+        <v>8</v>
+      </c>
+      <c r="D6" s="6">
+        <v>5.0800000000000001</v>
+      </c>
+      <c r="E6" s="6">
+        <v>1.22</v>
+      </c>
+      <c r="F6" s="8">
+        <v>86.5</v>
+      </c>
+      <c r="G6" s="6">
+        <f t="shared" si="0"/>
+        <v>2.54</v>
+      </c>
+      <c r="H6" s="6">
+        <f t="shared" si="1"/>
+        <v>2.54</v>
+      </c>
+      <c r="I6" s="8">
+        <v>0.80000000000000004</v>
+      </c>
+      <c r="J6" s="8">
+        <v>0.80000000000000004</v>
+      </c>
+      <c r="K6" s="8">
+        <v>1.5</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="2"/>
+        <v>0.40000000000000002</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="3"/>
+        <v>0.40000000000000002</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="8">
+        <v>16</v>
+      </c>
+      <c r="D7" s="6">
+        <v>5.0800000000000001</v>
+      </c>
+      <c r="E7" s="6">
+        <v>2.3399999999999999</v>
+      </c>
+      <c r="F7" s="8">
+        <v>66.200000000000003</v>
+      </c>
+      <c r="G7" s="6">
+        <f t="shared" si="0"/>
+        <v>2.54</v>
+      </c>
+      <c r="H7" s="6">
+        <f t="shared" si="1"/>
+        <v>2.54</v>
+      </c>
+      <c r="I7" s="8">
+        <v>0.80000000000000004</v>
+      </c>
+      <c r="J7" s="8">
+        <v>0.80000000000000004</v>
+      </c>
+      <c r="K7" s="8">
+        <v>1</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="2"/>
+        <v>0.40000000000000002</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="3"/>
+        <v>0.40000000000000002</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="8">
+        <v>32</v>
+      </c>
+      <c r="D8" s="6">
+        <v>5.0800000000000001</v>
+      </c>
+      <c r="E8" s="6">
+        <v>3.9399999999999999</v>
+      </c>
+      <c r="F8" s="8">
+        <v>40.200000000000003</v>
+      </c>
+      <c r="G8" s="6">
+        <f t="shared" si="0"/>
+        <v>2.54</v>
+      </c>
+      <c r="H8" s="6">
+        <f t="shared" si="1"/>
+        <v>2.54</v>
+      </c>
+      <c r="I8" s="8">
+        <v>0.80000000000000004</v>
+      </c>
+      <c r="J8" s="8">
+        <v>0.80000000000000004</v>
+      </c>
+      <c r="K8" s="8">
+        <v>1.5</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="2"/>
+        <v>0.40000000000000002</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="3"/>
+        <v>0.40000000000000002</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="8">
+        <v>64</v>
+      </c>
+      <c r="D9" s="6">
+        <v>5.1600000000000001</v>
+      </c>
+      <c r="E9" s="6">
+        <v>5</v>
+      </c>
+      <c r="F9" s="8">
+        <v>6.4000000000000004</v>
+      </c>
+      <c r="G9" s="6">
+        <f t="shared" si="0"/>
+        <v>2.5800000000000001</v>
+      </c>
+      <c r="H9" s="6">
+        <f t="shared" si="1"/>
+        <v>2.5800000000000001</v>
+      </c>
+      <c r="I9" s="8">
+        <v>0.80000000000000004</v>
+      </c>
+      <c r="J9" s="8">
+        <v>0.80000000000000004</v>
+      </c>
+      <c r="K9" s="8">
+        <v>1.5</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="2"/>
+        <v>0.40000000000000002</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="3"/>
+        <v>0.40000000000000002</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="8">
+        <v>128</v>
+      </c>
+      <c r="D10" s="6">
+        <v>5.1600000000000001</v>
+      </c>
+      <c r="E10" s="6">
+        <v>4.2800000000000002</v>
+      </c>
+      <c r="F10" s="8">
+        <v>-30</v>
+      </c>
+      <c r="G10" s="6">
+        <f t="shared" ref="G10:G17" si="4">D10/2</f>
+        <v>2.5800000000000001</v>
+      </c>
+      <c r="H10" s="6">
+        <f t="shared" ref="H10:H17" si="5">D10/2</f>
+        <v>2.5800000000000001</v>
+      </c>
+      <c r="I10" s="8">
+        <v>0.80000000000000004</v>
+      </c>
+      <c r="J10" s="8">
+        <v>0.80000000000000004</v>
+      </c>
+      <c r="K10" s="8">
+        <v>2</v>
+      </c>
+      <c r="L10">
+        <f t="shared" ref="L10:L17" si="6">I10/2</f>
+        <v>0.40000000000000002</v>
+      </c>
+      <c r="M10">
+        <f t="shared" ref="M10:M17" si="7">J10/2</f>
+        <v>0.40000000000000002</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="7"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="8">
+        <v>256</v>
+      </c>
+      <c r="D11" s="6">
+        <v>5.1600000000000001</v>
+      </c>
+      <c r="E11" s="6">
+        <v>2.6800000000000002</v>
+      </c>
+      <c r="F11" s="8">
+        <v>-56.299999999999997</v>
+      </c>
+      <c r="G11" s="6">
+        <f t="shared" si="4"/>
+        <v>2.5800000000000001</v>
+      </c>
+      <c r="H11" s="6">
+        <f t="shared" si="5"/>
+        <v>2.5800000000000001</v>
+      </c>
+      <c r="I11" s="8">
+        <v>0.80000000000000004</v>
+      </c>
+      <c r="J11" s="8">
+        <v>0.80000000000000004</v>
+      </c>
+      <c r="K11" s="8">
+        <v>2</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="6"/>
+        <v>0.40000000000000002</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="7"/>
+        <v>0.40000000000000002</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="7"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="8">
+        <v>512</v>
+      </c>
+      <c r="D12" s="6">
+        <v>5.1600000000000001</v>
+      </c>
+      <c r="E12" s="6">
+        <v>1.45</v>
+      </c>
+      <c r="F12" s="8">
+        <v>-70</v>
+      </c>
+      <c r="G12" s="6">
+        <f t="shared" si="4"/>
+        <v>2.5800000000000001</v>
+      </c>
+      <c r="H12" s="6">
+        <f t="shared" si="5"/>
+        <v>2.5800000000000001</v>
+      </c>
+      <c r="I12" s="8">
+        <v>0.80000000000000004</v>
+      </c>
+      <c r="J12" s="8">
+        <v>0.80000000000000004</v>
+      </c>
+      <c r="K12" s="8">
+        <v>2</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="6"/>
+        <v>0.40000000000000002</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="7"/>
+        <v>0.40000000000000002</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="8">
+        <v>1024</v>
+      </c>
+      <c r="D13" s="6">
+        <v>5.2000000000000002</v>
+      </c>
+      <c r="E13" s="6">
+        <v>0.75</v>
+      </c>
+      <c r="F13" s="8">
+        <v>-75.599999999999994</v>
+      </c>
+      <c r="G13" s="6">
+        <f t="shared" si="4"/>
+        <v>2.6000000000000001</v>
+      </c>
+      <c r="H13" s="6">
+        <f t="shared" si="5"/>
+        <v>2.6000000000000001</v>
+      </c>
+      <c r="I13" s="8">
+        <v>0.80000000000000004</v>
+      </c>
+      <c r="J13" s="8">
+        <v>0.80000000000000004</v>
+      </c>
+      <c r="K13" s="8">
+        <v>2</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="6"/>
+        <v>0.40000000000000002</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="7"/>
+        <v>0.40000000000000002</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="7"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="8">
+        <v>2048</v>
+      </c>
+      <c r="D14" s="6">
+        <v>5.2000000000000002</v>
+      </c>
+      <c r="E14" s="6">
+        <v>0.39000000000000001</v>
+      </c>
+      <c r="F14" s="8">
+        <v>-73.400000000000006</v>
+      </c>
+      <c r="G14" s="6">
+        <f t="shared" si="4"/>
+        <v>2.6000000000000001</v>
+      </c>
+      <c r="H14" s="6">
+        <f t="shared" si="5"/>
+        <v>2.6000000000000001</v>
+      </c>
+      <c r="I14" s="8">
+        <v>0.80000000000000004</v>
+      </c>
+      <c r="J14" s="8">
+        <v>0.80000000000000004</v>
+      </c>
+      <c r="K14" s="8">
+        <v>3</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="6"/>
+        <v>0.40000000000000002</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="7"/>
+        <v>0.40000000000000002</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="7"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="8">
+        <v>4096</v>
+      </c>
+      <c r="D15" s="6">
+        <v>5.2400000000000002</v>
+      </c>
+      <c r="E15" s="6">
+        <v>0.20999999999999999</v>
+      </c>
+      <c r="F15" s="8">
+        <v>-64</v>
+      </c>
+      <c r="G15" s="6">
+        <f t="shared" si="4"/>
+        <v>2.6200000000000001</v>
+      </c>
+      <c r="H15" s="6">
+        <f t="shared" si="5"/>
+        <v>2.6200000000000001</v>
+      </c>
+      <c r="I15" s="8">
+        <v>0.80000000000000004</v>
+      </c>
+      <c r="J15" s="8">
+        <v>0.80000000000000004</v>
+      </c>
+      <c r="K15" s="8">
+        <v>3</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="6"/>
+        <v>0.40000000000000002</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="7"/>
+        <v>0.40000000000000002</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="7"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="8">
+        <v>8192</v>
+      </c>
+      <c r="D16" s="6">
+        <v>5.2400000000000002</v>
+      </c>
+      <c r="E16" s="6">
+        <v>0.13</v>
+      </c>
+      <c r="F16" s="8">
+        <v>-50</v>
+      </c>
+      <c r="G16" s="6">
+        <f t="shared" si="4"/>
+        <v>2.6200000000000001</v>
+      </c>
+      <c r="H16" s="6">
+        <f t="shared" si="5"/>
+        <v>2.6200000000000001</v>
+      </c>
+      <c r="I16" s="8">
+        <v>0.80000000000000004</v>
+      </c>
+      <c r="J16" s="8">
+        <v>0.80000000000000004</v>
+      </c>
+      <c r="K16" s="8">
+        <v>4</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="6"/>
+        <v>0.40000000000000002</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="7"/>
+        <v>0.40000000000000002</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="7"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="8">
+        <v>16384</v>
+      </c>
+      <c r="D17" s="6">
+        <v>5.1600000000000001</v>
+      </c>
+      <c r="E17" s="6">
+        <v>0.089999999999999997</v>
+      </c>
+      <c r="F17" s="8">
+        <v>-31</v>
+      </c>
+      <c r="G17" s="6">
+        <f t="shared" si="4"/>
+        <v>2.5800000000000001</v>
+      </c>
+      <c r="H17" s="6">
+        <f t="shared" si="5"/>
+        <v>2.5800000000000001</v>
+      </c>
+      <c r="I17" s="8">
+        <v>0.80000000000000004</v>
+      </c>
+      <c r="J17" s="8">
+        <v>0.80000000000000004</v>
+      </c>
+      <c r="K17" s="8">
+        <v>3</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="6"/>
+        <v>0.40000000000000002</v>
+      </c>
+      <c r="M17">
+        <f t="shared" si="7"/>
+        <v>0.40000000000000002</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
terminata analisi dati (mancante solo revisione
</commit_message>
<xml_diff>
--- a/20240411circuiti3/circuiti3.xlsx
+++ b/20240411circuiti3/circuiti3.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t xml:space="preserve">R (kohm)</t>
   </si>
@@ -100,9 +100,6 @@
   </si>
   <si>
     <t>VLpp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">faseL  (deg)</t>
   </si>
   <si>
     <t>sigmaV_inpp</t>
@@ -4403,7 +4400,7 @@
         <v>27</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="G1" s="10" t="s">
         <v>2</v>
@@ -4412,10 +4409,10 @@
         <v>16</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>30</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>19</v>
@@ -4424,7 +4421,7 @@
         <v>11</v>
       </c>
       <c r="M1" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2">
@@ -4451,8 +4448,8 @@
         <v>2.54</v>
       </c>
       <c r="H2" s="6">
-        <f t="shared" ref="H2:H9" si="1">D2/2</f>
-        <v>2.54</v>
+        <f t="shared" ref="H2:H9" si="1">E2/2</f>
+        <v>0.012</v>
       </c>
       <c r="I2" s="8">
         <v>0.80000000000000004</v>
@@ -4463,11 +4460,11 @@
       <c r="K2" s="8">
         <v>3</v>
       </c>
-      <c r="L2">
+      <c r="L2" s="5">
         <f t="shared" ref="L2:L9" si="2">I2/2</f>
         <v>0.40000000000000002</v>
       </c>
-      <c r="M2">
+      <c r="M2" s="5">
         <f t="shared" ref="M2:M9" si="3">J2/2</f>
         <v>0.40000000000000002</v>
       </c>
@@ -4493,7 +4490,7 @@
       </c>
       <c r="H3" s="6">
         <f t="shared" si="1"/>
-        <v>2.54</v>
+        <v>0.040000000000000001</v>
       </c>
       <c r="I3" s="8">
         <v>0.80000000000000004</v>
@@ -4504,11 +4501,11 @@
       <c r="K3" s="8">
         <v>3</v>
       </c>
-      <c r="L3">
+      <c r="L3" s="5">
         <f t="shared" si="2"/>
         <v>0.40000000000000002</v>
       </c>
-      <c r="M3">
+      <c r="M3" s="5">
         <f t="shared" si="3"/>
         <v>0.40000000000000002</v>
       </c>
@@ -4534,7 +4531,7 @@
       </c>
       <c r="H4" s="6">
         <f t="shared" si="1"/>
-        <v>2.54</v>
+        <v>0.12</v>
       </c>
       <c r="I4" s="8">
         <v>0.80000000000000004</v>
@@ -4545,11 +4542,11 @@
       <c r="K4" s="8">
         <v>3</v>
       </c>
-      <c r="L4">
+      <c r="L4" s="5">
         <f t="shared" si="2"/>
         <v>0.40000000000000002</v>
       </c>
-      <c r="M4">
+      <c r="M4" s="5">
         <f t="shared" si="3"/>
         <v>0.40000000000000002</v>
       </c>
@@ -4575,7 +4572,7 @@
       </c>
       <c r="H5" s="6">
         <f t="shared" si="1"/>
-        <v>2.54</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="I5" s="8">
         <v>0.80000000000000004</v>
@@ -4586,11 +4583,11 @@
       <c r="K5" s="8">
         <v>2</v>
       </c>
-      <c r="L5">
+      <c r="L5" s="5">
         <f t="shared" si="2"/>
         <v>0.40000000000000002</v>
       </c>
-      <c r="M5">
+      <c r="M5" s="5">
         <f t="shared" si="3"/>
         <v>0.40000000000000002</v>
       </c>
@@ -4616,7 +4613,7 @@
       </c>
       <c r="H6" s="6">
         <f t="shared" si="1"/>
-        <v>2.54</v>
+        <v>0.60999999999999999</v>
       </c>
       <c r="I6" s="8">
         <v>0.80000000000000004</v>
@@ -4627,11 +4624,11 @@
       <c r="K6" s="8">
         <v>1.5</v>
       </c>
-      <c r="L6">
+      <c r="L6" s="5">
         <f t="shared" si="2"/>
         <v>0.40000000000000002</v>
       </c>
-      <c r="M6">
+      <c r="M6" s="5">
         <f t="shared" si="3"/>
         <v>0.40000000000000002</v>
       </c>
@@ -4657,7 +4654,7 @@
       </c>
       <c r="H7" s="6">
         <f t="shared" si="1"/>
-        <v>2.54</v>
+        <v>1.1699999999999999</v>
       </c>
       <c r="I7" s="8">
         <v>0.80000000000000004</v>
@@ -4668,11 +4665,11 @@
       <c r="K7" s="8">
         <v>1</v>
       </c>
-      <c r="L7">
+      <c r="L7" s="5">
         <f t="shared" si="2"/>
         <v>0.40000000000000002</v>
       </c>
-      <c r="M7">
+      <c r="M7" s="5">
         <f t="shared" si="3"/>
         <v>0.40000000000000002</v>
       </c>
@@ -4698,7 +4695,7 @@
       </c>
       <c r="H8" s="6">
         <f t="shared" si="1"/>
-        <v>2.54</v>
+        <v>1.97</v>
       </c>
       <c r="I8" s="8">
         <v>0.80000000000000004</v>
@@ -4709,11 +4706,11 @@
       <c r="K8" s="8">
         <v>1.5</v>
       </c>
-      <c r="L8">
+      <c r="L8" s="5">
         <f t="shared" si="2"/>
         <v>0.40000000000000002</v>
       </c>
-      <c r="M8">
+      <c r="M8" s="5">
         <f t="shared" si="3"/>
         <v>0.40000000000000002</v>
       </c>
@@ -4739,7 +4736,7 @@
       </c>
       <c r="H9" s="6">
         <f t="shared" si="1"/>
-        <v>2.5800000000000001</v>
+        <v>2.5</v>
       </c>
       <c r="I9" s="8">
         <v>0.80000000000000004</v>
@@ -4750,11 +4747,11 @@
       <c r="K9" s="8">
         <v>1.5</v>
       </c>
-      <c r="L9">
+      <c r="L9" s="5">
         <f t="shared" si="2"/>
         <v>0.40000000000000002</v>
       </c>
-      <c r="M9">
+      <c r="M9" s="5">
         <f t="shared" si="3"/>
         <v>0.40000000000000002</v>
       </c>
@@ -4779,8 +4776,8 @@
         <v>2.5800000000000001</v>
       </c>
       <c r="H10" s="6">
-        <f t="shared" ref="H10:H17" si="5">D10/2</f>
-        <v>2.5800000000000001</v>
+        <f t="shared" ref="H10:H17" si="5">E10/2</f>
+        <v>2.1400000000000001</v>
       </c>
       <c r="I10" s="8">
         <v>0.80000000000000004</v>
@@ -4791,11 +4788,11 @@
       <c r="K10" s="8">
         <v>2</v>
       </c>
-      <c r="L10">
+      <c r="L10" s="5">
         <f t="shared" ref="L10:L17" si="6">I10/2</f>
         <v>0.40000000000000002</v>
       </c>
-      <c r="M10">
+      <c r="M10" s="5">
         <f t="shared" ref="M10:M17" si="7">J10/2</f>
         <v>0.40000000000000002</v>
       </c>
@@ -4821,7 +4818,7 @@
       </c>
       <c r="H11" s="6">
         <f t="shared" si="5"/>
-        <v>2.5800000000000001</v>
+        <v>1.3400000000000001</v>
       </c>
       <c r="I11" s="8">
         <v>0.80000000000000004</v>
@@ -4832,11 +4829,11 @@
       <c r="K11" s="8">
         <v>2</v>
       </c>
-      <c r="L11">
+      <c r="L11" s="5">
         <f t="shared" si="6"/>
         <v>0.40000000000000002</v>
       </c>
-      <c r="M11">
+      <c r="M11" s="5">
         <f t="shared" si="7"/>
         <v>0.40000000000000002</v>
       </c>
@@ -4862,7 +4859,7 @@
       </c>
       <c r="H12" s="6">
         <f t="shared" si="5"/>
-        <v>2.5800000000000001</v>
+        <v>0.72499999999999998</v>
       </c>
       <c r="I12" s="8">
         <v>0.80000000000000004</v>
@@ -4873,11 +4870,11 @@
       <c r="K12" s="8">
         <v>2</v>
       </c>
-      <c r="L12">
+      <c r="L12" s="5">
         <f t="shared" si="6"/>
         <v>0.40000000000000002</v>
       </c>
-      <c r="M12">
+      <c r="M12" s="5">
         <f t="shared" si="7"/>
         <v>0.40000000000000002</v>
       </c>
@@ -4903,7 +4900,7 @@
       </c>
       <c r="H13" s="6">
         <f t="shared" si="5"/>
-        <v>2.6000000000000001</v>
+        <v>0.375</v>
       </c>
       <c r="I13" s="8">
         <v>0.80000000000000004</v>
@@ -4914,11 +4911,11 @@
       <c r="K13" s="8">
         <v>2</v>
       </c>
-      <c r="L13">
+      <c r="L13" s="5">
         <f t="shared" si="6"/>
         <v>0.40000000000000002</v>
       </c>
-      <c r="M13">
+      <c r="M13" s="5">
         <f t="shared" si="7"/>
         <v>0.40000000000000002</v>
       </c>
@@ -4944,7 +4941,7 @@
       </c>
       <c r="H14" s="6">
         <f t="shared" si="5"/>
-        <v>2.6000000000000001</v>
+        <v>0.19500000000000001</v>
       </c>
       <c r="I14" s="8">
         <v>0.80000000000000004</v>
@@ -4955,11 +4952,11 @@
       <c r="K14" s="8">
         <v>3</v>
       </c>
-      <c r="L14">
+      <c r="L14" s="5">
         <f t="shared" si="6"/>
         <v>0.40000000000000002</v>
       </c>
-      <c r="M14">
+      <c r="M14" s="5">
         <f t="shared" si="7"/>
         <v>0.40000000000000002</v>
       </c>
@@ -4985,7 +4982,7 @@
       </c>
       <c r="H15" s="6">
         <f t="shared" si="5"/>
-        <v>2.6200000000000001</v>
+        <v>0.105</v>
       </c>
       <c r="I15" s="8">
         <v>0.80000000000000004</v>
@@ -4996,11 +4993,11 @@
       <c r="K15" s="8">
         <v>3</v>
       </c>
-      <c r="L15">
+      <c r="L15" s="5">
         <f t="shared" si="6"/>
         <v>0.40000000000000002</v>
       </c>
-      <c r="M15">
+      <c r="M15" s="5">
         <f t="shared" si="7"/>
         <v>0.40000000000000002</v>
       </c>
@@ -5026,7 +5023,7 @@
       </c>
       <c r="H16" s="6">
         <f t="shared" si="5"/>
-        <v>2.6200000000000001</v>
+        <v>0.065000000000000002</v>
       </c>
       <c r="I16" s="8">
         <v>0.80000000000000004</v>
@@ -5037,11 +5034,11 @@
       <c r="K16" s="8">
         <v>4</v>
       </c>
-      <c r="L16">
+      <c r="L16" s="5">
         <f t="shared" si="6"/>
         <v>0.40000000000000002</v>
       </c>
-      <c r="M16">
+      <c r="M16" s="5">
         <f t="shared" si="7"/>
         <v>0.40000000000000002</v>
       </c>
@@ -5067,7 +5064,7 @@
       </c>
       <c r="H17" s="6">
         <f t="shared" si="5"/>
-        <v>2.5800000000000001</v>
+        <v>0.044999999999999998</v>
       </c>
       <c r="I17" s="8">
         <v>0.80000000000000004</v>
@@ -5078,11 +5075,11 @@
       <c r="K17" s="8">
         <v>3</v>
       </c>
-      <c r="L17">
+      <c r="L17" s="5">
         <f t="shared" si="6"/>
         <v>0.40000000000000002</v>
       </c>
-      <c r="M17">
+      <c r="M17" s="5">
         <f t="shared" si="7"/>
         <v>0.40000000000000002</v>
       </c>

</xml_diff>